<commit_message>
Validation of 2a-b & refining input space of 2b
</commit_message>
<xml_diff>
--- a/General/Def1a - variable selection.xlsx
+++ b/General/Def1a - variable selection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://firstrandgroup-my.sharepoint.com/personal/wrq_rmb_co_za/Documents/Analytix/Research/Dynamic SICR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkLife\Analytix\Research\Dynamic-SICR\IFRS9-SICR-Definitions-Logit\General\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="13_ncr:1_{FFDDFC6F-4CD5-4B27-ABD0-0321AC4D99C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0334022E-C165-4DF7-B781-19ECA64D6130}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA0D76A-9749-43E2-AA2F-23E40B81BF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9D6FC385-DBE1-4183-BFCB-3D03C3BB241A}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="27180" windowHeight="18885" xr2:uid="{9D6FC385-DBE1-4183-BFCB-3D03C3BB241A}"/>
   </bookViews>
   <sheets>
     <sheet name="Account-level" sheetId="1" r:id="rId1"/>
@@ -113,12 +113,6 @@
     <t>X marks whether or not an input was statistically significant at 5% level after interactive selection process</t>
   </si>
   <si>
-    <t>Green-shade cells marks final inclusion as input in 'standardisation' the input space</t>
-  </si>
-  <si>
-    <t>slc_pmnt_method*</t>
-  </si>
-  <si>
     <t>slc_acct_pre_lim_perc_imputed</t>
   </si>
   <si>
@@ -171,13 +165,19 @@
   </si>
   <si>
     <t>Real income</t>
+  </si>
+  <si>
+    <t>Green-shade cells marks final inclusion as input in 'standardisation' of the input space</t>
+  </si>
+  <si>
+    <t>slc_pmnt_method</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,9 +253,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -277,7 +274,7 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -298,9 +295,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -338,7 +335,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -444,7 +441,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -586,7 +583,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -597,10 +594,10 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A13"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
@@ -617,7 +614,7 @@
     <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -664,7 +661,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -695,7 +692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -720,7 +717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -749,7 +746,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -778,7 +775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -807,7 +804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -836,7 +833,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -863,17 +860,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -886,10 +883,10 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
@@ -905,21 +902,21 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -931,7 +928,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -943,7 +940,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -955,7 +952,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -969,7 +966,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -983,7 +980,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -997,7 +994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1023,7 +1020,7 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -1042,36 +1039,36 @@
     <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1095,7 +1092,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1119,7 +1116,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1143,7 +1140,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1169,7 +1166,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1195,7 +1192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1221,7 +1218,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1259,43 +1256,43 @@
       <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:15">
+        <v>34</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="13"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="7">
+      <c r="B2" s="13">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="7">
+      <c r="I2" s="13">
         <v>12</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1342,169 +1339,169 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="5" t="s">
+      <c r="B6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="5" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="2" t="s">
+      <c r="B8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>